<commit_message>
Implemented a basic navigator for UserAccessActivity.kt LoginFragment.kt  : The function argument was causing errors with
</commit_message>
<xml_diff>
--- a/Measures for App.xlsx
+++ b/Measures for App.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Dropbox\CSProject\BootCampAndroid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BB69626-6333-48EA-A106-012699F3B98B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51000561-45F8-4145-ABD5-4711D45E353F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D67FF71C-EB35-4F88-BE45-37DEE527D0C6}"/>
+    <workbookView xWindow="510" yWindow="1570" windowWidth="13030" windowHeight="7360" xr2:uid="{D67FF71C-EB35-4F88-BE45-37DEE527D0C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Height</t>
   </si>
@@ -107,10 +106,13 @@
     <t>Device Dp</t>
   </si>
   <si>
-    <t>Padding login</t>
-  </si>
-  <si>
     <t>Padding Loggin Field</t>
+  </si>
+  <si>
+    <t>Registration icon height</t>
+  </si>
+  <si>
+    <t>Registration icon width</t>
   </si>
 </sst>
 </file>
@@ -465,14 +467,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C62D0E05-E872-4BB2-A8A8-9C3493BE9D26}">
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="30.1796875" customWidth="1"/>
     <col min="5" max="5" width="8.7265625" style="2"/>
     <col min="6" max="6" width="11.36328125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.81640625" bestFit="1" customWidth="1"/>
@@ -582,14 +585,14 @@
         <v>1075</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D13" si="0">B3/C3</f>
+        <f t="shared" ref="D3:D15" si="0">B3/C3</f>
         <v>1.5813953488372091E-2</v>
       </c>
       <c r="E3" s="3">
         <v>891</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F13" si="1">D3*E3</f>
+        <f t="shared" ref="F3:F15" si="1">D3*E3</f>
         <v>14.090232558139533</v>
       </c>
       <c r="H3" t="s">
@@ -646,7 +649,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5">
         <v>64</v>
@@ -848,9 +851,47 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="B14">
+        <v>71</v>
+      </c>
+      <c r="C14">
+        <v>928</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>7.6508620689655166E-2</v>
+      </c>
+      <c r="E14" s="3">
+        <v>891</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" si="1"/>
+        <v>68.169181034482747</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15">
+        <v>141</v>
+      </c>
+      <c r="C15">
+        <v>436</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>0.32339449541284404</v>
+      </c>
+      <c r="E15" s="3">
+        <v>411</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" si="1"/>
+        <v>132.91513761467891</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Set styles and better UI for fragments
</commit_message>
<xml_diff>
--- a/Measures for App.xlsx
+++ b/Measures for App.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Dropbox\CSProject\BootCampAndroid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51000561-45F8-4145-ABD5-4711D45E353F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D1FF1D-B279-401D-AB61-2B1F0EB2C8BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="1570" windowWidth="13030" windowHeight="7360" xr2:uid="{D67FF71C-EB35-4F88-BE45-37DEE527D0C6}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="7270" xr2:uid="{D67FF71C-EB35-4F88-BE45-37DEE527D0C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>Height</t>
   </si>
@@ -113,6 +113,15 @@
   </si>
   <si>
     <t>Registration icon width</t>
+  </si>
+  <si>
+    <t>Registration margin left</t>
+  </si>
+  <si>
+    <t>Registration top margin text field</t>
+  </si>
+  <si>
+    <t>Registration top margin text view</t>
   </si>
 </sst>
 </file>
@@ -467,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C62D0E05-E872-4BB2-A8A8-9C3493BE9D26}">
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -585,14 +594,14 @@
         <v>1075</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D15" si="0">B3/C3</f>
+        <f t="shared" ref="D3:D17" si="0">B3/C3</f>
         <v>1.5813953488372091E-2</v>
       </c>
       <c r="E3" s="3">
         <v>891</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F15" si="1">D3*E3</f>
+        <f t="shared" ref="F3:F17" si="1">D3*E3</f>
         <v>14.090232558139533</v>
       </c>
       <c r="H3" t="s">
@@ -891,6 +900,94 @@
       <c r="F15" s="2">
         <f t="shared" si="1"/>
         <v>132.91513761467891</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16">
+        <v>54</v>
+      </c>
+      <c r="C16">
+        <v>910</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>5.9340659340659338E-2</v>
+      </c>
+      <c r="E16" s="3">
+        <v>411</v>
+      </c>
+      <c r="F16" s="2">
+        <f t="shared" si="1"/>
+        <v>24.389010989010988</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17">
+        <v>26</v>
+      </c>
+      <c r="C17">
+        <v>944</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>2.7542372881355932E-2</v>
+      </c>
+      <c r="E17" s="2">
+        <v>891</v>
+      </c>
+      <c r="F17" s="2">
+        <f t="shared" si="1"/>
+        <v>24.540254237288135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18">
+        <v>50</v>
+      </c>
+      <c r="C18">
+        <v>944</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" ref="D18" si="2">B18/C18</f>
+        <v>5.2966101694915252E-2</v>
+      </c>
+      <c r="E18" s="2">
+        <v>891</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="shared" ref="F18" si="3">D18*E18</f>
+        <v>47.192796610169488</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>944</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" ref="D19" si="4">B19/C19</f>
+        <v>1.8008474576271187E-2</v>
+      </c>
+      <c r="E19" s="2">
+        <v>891</v>
+      </c>
+      <c r="F19" s="2">
+        <f t="shared" ref="F19" si="5">D19*E19</f>
+        <v>16.045550847457626</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated item_recomendation_movie.xml and nonexistent elements trying to bind in MovieRecomendationViewHolder.kt
</commit_message>
<xml_diff>
--- a/Measures for App.xlsx
+++ b/Measures for App.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Dropbox\CSProject\BootCampAndroid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D1FF1D-B279-401D-AB61-2B1F0EB2C8BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF56766B-961D-4D8B-9653-21CDF1808197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="7270" xr2:uid="{D67FF71C-EB35-4F88-BE45-37DEE527D0C6}"/>
+    <workbookView xWindow="5600" yWindow="2400" windowWidth="14400" windowHeight="7270" xr2:uid="{D67FF71C-EB35-4F88-BE45-37DEE527D0C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
   <si>
     <t>Height</t>
   </si>
@@ -122,6 +122,39 @@
   </si>
   <si>
     <t>Registration top margin text view</t>
+  </si>
+  <si>
+    <t>Recommended movie layout width</t>
+  </si>
+  <si>
+    <t>Recommended movie layout height</t>
+  </si>
+  <si>
+    <t>Recommended movie image height</t>
+  </si>
+  <si>
+    <t>Recommended movie rating image height</t>
+  </si>
+  <si>
+    <t>Recommended movie marginstart rating to rating image</t>
+  </si>
+  <si>
+    <t>Recommended movie margintop rating to thumbnail</t>
+  </si>
+  <si>
+    <t>Recommended movie marginstart rating image to parent</t>
+  </si>
+  <si>
+    <t>Recommended movie Rating text height</t>
+  </si>
+  <si>
+    <t>Recommended movie margintop moviename to ratingimage</t>
+  </si>
+  <si>
+    <t>Recommended movie marginstart layout to parent</t>
+  </si>
+  <si>
+    <t>Recommended movie marginend layout to parent</t>
   </si>
 </sst>
 </file>
@@ -476,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C62D0E05-E872-4BB2-A8A8-9C3493BE9D26}">
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -979,15 +1012,345 @@
         <v>944</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" ref="D19" si="4">B19/C19</f>
+        <f t="shared" ref="D19:D21" si="4">B19/C19</f>
         <v>1.8008474576271187E-2</v>
       </c>
       <c r="E19" s="2">
         <v>891</v>
       </c>
       <c r="F19" s="2">
-        <f t="shared" ref="F19" si="5">D19*E19</f>
+        <f t="shared" ref="F19:F21" si="5">D19*E19</f>
         <v>16.045550847457626</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20">
+        <v>150</v>
+      </c>
+      <c r="C20">
+        <v>493</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="4"/>
+        <v>0.30425963488843816</v>
+      </c>
+      <c r="E20" s="3">
+        <v>411</v>
+      </c>
+      <c r="F20" s="2">
+        <f t="shared" si="5"/>
+        <v>125.05070993914808</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21">
+        <v>309</v>
+      </c>
+      <c r="C21">
+        <v>997</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="4"/>
+        <v>0.30992978936810434</v>
+      </c>
+      <c r="E21" s="2">
+        <v>891</v>
+      </c>
+      <c r="F21" s="2">
+        <f t="shared" si="5"/>
+        <v>276.14744232698098</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22">
+        <v>218</v>
+      </c>
+      <c r="C22">
+        <v>997</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" ref="D22" si="6">B22/C22</f>
+        <v>0.21865596790371114</v>
+      </c>
+      <c r="E22" s="2">
+        <v>891</v>
+      </c>
+      <c r="F22" s="2">
+        <f t="shared" ref="F22" si="7">D22*E22</f>
+        <v>194.82246740220663</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23">
+        <v>218</v>
+      </c>
+      <c r="C23">
+        <v>997</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" ref="D23" si="8">B23/C23</f>
+        <v>0.21865596790371114</v>
+      </c>
+      <c r="E23" s="2">
+        <v>891</v>
+      </c>
+      <c r="F23" s="2">
+        <f t="shared" ref="F23" si="9">D23*E23</f>
+        <v>194.82246740220663</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24">
+        <v>13</v>
+      </c>
+      <c r="C24">
+        <v>997</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" ref="D24" si="10">B24/C24</f>
+        <v>1.3039117352056168E-2</v>
+      </c>
+      <c r="E24" s="2">
+        <v>891</v>
+      </c>
+      <c r="F24" s="2">
+        <f t="shared" ref="F24" si="11">D24*E24</f>
+        <v>11.617853560682047</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>997</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" ref="D25" si="12">B25/C25</f>
+        <v>8.0240722166499499E-3</v>
+      </c>
+      <c r="E25" s="2">
+        <v>891</v>
+      </c>
+      <c r="F25" s="2">
+        <f t="shared" ref="F25" si="13">D25*E25</f>
+        <v>7.149448345035105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26">
+        <v>16</v>
+      </c>
+      <c r="C26">
+        <v>997</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" ref="D26:D27" si="14">B26/C26</f>
+        <v>1.60481444332999E-2</v>
+      </c>
+      <c r="E26" s="2">
+        <v>891</v>
+      </c>
+      <c r="F26" s="2">
+        <f t="shared" ref="F26:F27" si="15">D26*E26</f>
+        <v>14.29889669007021</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>493</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="14"/>
+        <v>1.6227180527383367E-2</v>
+      </c>
+      <c r="E27" s="3">
+        <v>411</v>
+      </c>
+      <c r="F27" s="2">
+        <f t="shared" si="15"/>
+        <v>6.6693711967545637</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28">
+        <v>12</v>
+      </c>
+      <c r="C28">
+        <v>997</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" ref="D28:D29" si="16">B28/C28</f>
+        <v>1.2036108324974924E-2</v>
+      </c>
+      <c r="E28" s="2">
+        <v>891</v>
+      </c>
+      <c r="F28" s="2">
+        <f t="shared" ref="F28:F29" si="17">D28*E28</f>
+        <v>10.724172517552658</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29">
+        <v>14</v>
+      </c>
+      <c r="C29">
+        <v>493</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="16"/>
+        <v>2.8397565922920892E-2</v>
+      </c>
+      <c r="E29" s="3">
+        <v>411</v>
+      </c>
+      <c r="F29" s="2">
+        <f t="shared" si="17"/>
+        <v>11.671399594320487</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30">
+        <v>12</v>
+      </c>
+      <c r="C30">
+        <v>997</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" ref="D30:D32" si="18">B30/C30</f>
+        <v>1.2036108324974924E-2</v>
+      </c>
+      <c r="E30" s="2">
+        <v>891</v>
+      </c>
+      <c r="F30" s="2">
+        <f t="shared" ref="F30:F32" si="19">D30*E30</f>
+        <v>10.724172517552658</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <v>493</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="18"/>
+        <v>1.0141987829614604E-2</v>
+      </c>
+      <c r="E31" s="3">
+        <v>411</v>
+      </c>
+      <c r="F31" s="2">
+        <f t="shared" si="19"/>
+        <v>4.1683569979716024</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32">
+        <v>30</v>
+      </c>
+      <c r="C32">
+        <v>493</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" si="18"/>
+        <v>6.0851926977687626E-2</v>
+      </c>
+      <c r="E32" s="3">
+        <v>411</v>
+      </c>
+      <c r="F32" s="2">
+        <f t="shared" si="19"/>
+        <v>25.010141987829613</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33">
+        <v>25</v>
+      </c>
+      <c r="C33">
+        <v>493</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" ref="D33:D34" si="20">B33/C33</f>
+        <v>5.0709939148073022E-2</v>
+      </c>
+      <c r="E33" s="3">
+        <v>411</v>
+      </c>
+      <c r="F33" s="2">
+        <f t="shared" ref="F33:F34" si="21">D33*E33</f>
+        <v>20.841784989858013</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34">
+        <v>47</v>
+      </c>
+      <c r="C34">
+        <v>997</v>
+      </c>
+      <c r="D34" s="1">
+        <f t="shared" si="20"/>
+        <v>4.7141424272818457E-2</v>
+      </c>
+      <c r="E34" s="2">
+        <v>891</v>
+      </c>
+      <c r="F34" s="2">
+        <f t="shared" si="21"/>
+        <v>42.003009027081248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented a search filter in MoviesViewModel.kt that  SearchFragment.kt uses
</commit_message>
<xml_diff>
--- a/Measures for App.xlsx
+++ b/Measures for App.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Dropbox\CSProject\BootCampAndroid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47ADB900-E11A-4597-B4D2-B1BDFAB80B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7165F9AD-9CC8-4FE9-9BA7-2ED39242B4E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5600" yWindow="2400" windowWidth="14400" windowHeight="7270" xr2:uid="{D67FF71C-EB35-4F88-BE45-37DEE527D0C6}"/>
   </bookViews>
@@ -533,7 +533,7 @@
   <dimension ref="A1:Q41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>